<commit_message>
Added Test Selecion page, splash screen, singel test feedback
</commit_message>
<xml_diff>
--- a/data_raw/SMT_dict.xlsx
+++ b/data_raw/SMT_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\packages\SMT\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BF301E-6389-44E6-B6D9-B072BDA8AE3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90964D9-416C-46E7-992E-6123A3FC9F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="171">
   <si>
     <t>key</t>
   </si>
@@ -515,6 +515,24 @@
   </si>
   <si>
     <t>en</t>
+  </si>
+  <si>
+    <t>TEST_SELECTION</t>
+  </si>
+  <si>
+    <t>Bitte wähle die Aufgabengruppen und die gewünschte Fragenanzahl (Tonhöhe ist immer dabei).</t>
+  </si>
+  <si>
+    <t>Please select task group and item numbers (PITCH is always included)</t>
+  </si>
+  <si>
+    <t>SCORE_HEADER_SINGLE</t>
+  </si>
+  <si>
+    <t>Ergebnis in der  Aufgabengruppe '{{task_group}}': {{result}}</t>
+  </si>
+  <si>
+    <t>Your score in the  task group '{{task_group}}': {{result}}</t>
   </si>
 </sst>
 </file>
@@ -995,10 +1013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1222,499 +1240,522 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>20</v>
+        <v>169</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>161</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="11" t="s">
-        <v>13</v>
+        <v>158</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>28</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B23" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C23" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="75">
-      <c r="A23" s="13" t="s">
+    <row r="24" spans="1:5" ht="75">
+      <c r="A24" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B24" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C24" s="10" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="75">
-      <c r="A24" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" ht="75">
       <c r="A25" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>105</v>
+        <v>68</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>106</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" ht="75">
       <c r="A26" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="75">
+      <c r="A27" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B27" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C27" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="107.1" customHeight="1">
-      <c r="A27" s="11" t="s">
+    <row r="28" spans="1:5" ht="107.1" customHeight="1">
+      <c r="A28" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B28" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C28" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:5" ht="174" customHeight="1">
-      <c r="A28" s="11" t="s">
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" ht="174" customHeight="1">
+      <c r="A29" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B29" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C29" s="9" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="11" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>140</v>
+        <v>84</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>162</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>89</v>
+        <v>133</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>90</v>
+        <v>134</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="11" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="11" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="11" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="11" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>129</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
+        <v>128</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C52">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B53">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C53">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B54">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C54">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B55">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C55">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B56" t="s">
-        <v>49</v>
-      </c>
-      <c r="C56" t="s">
-        <v>147</v>
+        <v>139</v>
+      </c>
+      <c r="B56">
+        <v>5</v>
+      </c>
+      <c r="C56">
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B57" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C57" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B58" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C58" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B59" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C59" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B60" t="s">
-        <v>157</v>
+        <v>51</v>
       </c>
       <c r="C60" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B61" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C61" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="11" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="B62" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C62" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="11" t="s">
-        <v>154</v>
+        <v>6</v>
       </c>
       <c r="B63" t="s">
         <v>155</v>
       </c>
       <c r="C63" t="s">
         <v>156</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B64" t="s">
+        <v>155</v>
+      </c>
+      <c r="C64" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B65" t="s">
+        <v>166</v>
+      </c>
+      <c r="C65" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>